<commit_message>
morphology FP for whole catchment mix-2024
</commit_message>
<xml_diff>
--- a/all_data/DON_FP_2020-2021.xlsx
+++ b/all_data/DON_FP_2020-2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -1114,8 +1114,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK28" sqref="AK28:AK29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4145,8 +4146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F42" sqref="F42"/>

</xml_diff>